<commit_message>
feat: Implement filtering options for employee data
</commit_message>
<xml_diff>
--- a/backend/public/pranay.xlsx
+++ b/backend/public/pranay.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>EmployeeId</t>
   </si>
@@ -41,28 +41,10 @@
     <t>active</t>
   </si>
   <si>
-    <t>12th September2020</t>
-  </si>
-  <si>
     <t>React</t>
   </si>
   <si>
     <t>kota</t>
-  </si>
-  <si>
-    <t>13th September2020</t>
-  </si>
-  <si>
-    <t>14th September2020</t>
-  </si>
-  <si>
-    <t>15th September2020</t>
-  </si>
-  <si>
-    <t>16th September2020</t>
-  </si>
-  <si>
-    <t>17th September2020</t>
   </si>
   <si>
     <t>Rawat</t>
@@ -130,7 +112,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,7 +405,7 @@
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -437,20 +419,20 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>18</v>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -463,20 +445,20 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
+      <c r="D2" s="1">
+        <v>45211</v>
       </c>
       <c r="E2" s="1">
         <v>36078</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <v>20000</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -484,25 +466,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
+      <c r="D3" s="1">
+        <v>41559</v>
       </c>
       <c r="E3" s="1">
         <v>36079</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3">
         <v>20001</v>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -510,25 +492,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
+      <c r="D4" s="1">
+        <v>41559</v>
       </c>
       <c r="E4" s="1">
         <v>36080</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G4">
         <v>20002</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -536,25 +518,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
+      <c r="D5" s="1">
+        <v>41559</v>
       </c>
       <c r="E5" s="1">
         <v>36081</v>
       </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G5">
         <v>20003</v>
       </c>
       <c r="H5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -562,25 +544,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
-        <v>11</v>
+      <c r="D6" s="1">
+        <v>41559</v>
       </c>
       <c r="E6" s="1">
         <v>36082</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <v>20004</v>
       </c>
       <c r="H6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -588,28 +570,40 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
-        <v>12</v>
+      <c r="D7" s="1">
+        <v>41559</v>
       </c>
       <c r="E7" s="1">
         <v>36083</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <v>20005</v>
       </c>
       <c r="H7" t="s">
-        <v>7</v>
-      </c>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix- duplicate data insertion in mongodb
</commit_message>
<xml_diff>
--- a/backend/public/pranay.xlsx
+++ b/backend/public/pranay.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>EmployeeId</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>address</t>
+  </si>
+  <si>
+    <t>inactive</t>
+  </si>
+  <si>
+    <t>Kota</t>
   </si>
 </sst>
 </file>
@@ -395,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +452,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1">
-        <v>45211</v>
+        <v>45212</v>
       </c>
       <c r="E2" s="1">
         <v>36078</v>
@@ -592,12 +598,56 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45211</v>
+      </c>
+      <c r="E8" s="1">
+        <v>41197</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>20005</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45211</v>
+      </c>
+      <c r="E9" s="1">
+        <v>41197</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>20006</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E10" s="1"/>

</xml_diff>